<commit_message>
first attemp of size dependent consumption
</commit_message>
<xml_diff>
--- a/OptimSize.xlsx
+++ b/OptimSize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Size_Consumption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36093F29-FE68-48B5-944A-D42E1C6F0EDC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA5E9D9-6C78-4A80-B131-A84BCCC9847D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A77FD14E-277F-4AE2-BBD9-FAE0E9C9CB9C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Oithona davisae</t>
   </si>
@@ -106,6 +106,48 @@
   </si>
   <si>
     <t>https://doi.org/10.1093/plankt/1.4.313</t>
+  </si>
+  <si>
+    <t>Calaniod</t>
+  </si>
+  <si>
+    <t>Oithonid</t>
+  </si>
+  <si>
+    <t>Corycaeid</t>
+  </si>
+  <si>
+    <t>Oncaeid</t>
+  </si>
+  <si>
+    <t>Harpacticoid</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>HN</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1163/193724097X00179</t>
+  </si>
+  <si>
+    <t>Naupliar Development of Tigriopus japonicus Mori, 1932 (Copepoda: Harpacticidae)</t>
+  </si>
+  <si>
+    <t>conversion</t>
+  </si>
+  <si>
+    <t>doi:10.6620/ZS.2017.56-13</t>
   </si>
 </sst>
 </file>
@@ -150,10 +192,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -469,15 +512,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EF37AE-1B1C-479B-B90C-A1B96650C98F}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -558,7 +602,7 @@
       <c r="E5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -589,10 +633,10 @@
       <c r="E7">
         <v>0.04</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -616,11 +660,180 @@
         <v>24</v>
       </c>
     </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>237</v>
+      </c>
+      <c r="C18">
+        <v>165</v>
+      </c>
+      <c r="D18">
+        <v>85</v>
+      </c>
+      <c r="E18">
+        <v>85</v>
+      </c>
+      <c r="F18">
+        <v>133</v>
+      </c>
+      <c r="H18">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19">
+        <v>106</v>
+      </c>
+      <c r="E19">
+        <v>106</v>
+      </c>
+      <c r="F19">
+        <v>156</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>132</v>
+      </c>
+      <c r="E20">
+        <v>132</v>
+      </c>
+      <c r="F20">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>155</v>
+      </c>
+      <c r="E21">
+        <v>155</v>
+      </c>
+      <c r="F21">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>182</v>
+      </c>
+      <c r="E22">
+        <v>182</v>
+      </c>
+      <c r="F22">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>217</v>
+      </c>
+      <c r="E23">
+        <v>217</v>
+      </c>
+      <c r="F23">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>237</v>
+      </c>
+      <c r="C26">
+        <v>165</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE(D18:D22)</f>
+        <v>132</v>
+      </c>
+      <c r="E26">
+        <f>AVERAGE(E18:E22)</f>
+        <v>132</v>
+      </c>
+      <c r="F26">
+        <f>AVERAGE(F18:F20)</f>
+        <v>159</v>
+      </c>
+      <c r="G26">
+        <v>237</v>
+      </c>
+      <c r="H26">
+        <v>109</v>
+      </c>
+      <c r="I26">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{7D543D0F-5746-409A-A27D-1FF5C76FA0C5}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{F0E35FD9-0C18-4705-BE3B-B6406EC25791}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{58172047-CD7A-43C7-BED8-B0931C394ED5}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{97EFC8BD-C7B2-4A4C-AC80-C657F3781398}"/>
+    <hyperlink ref="B19" r:id="rId5" xr:uid="{A96D1FC8-7962-4284-9FFD-EE98DAF3446D}"/>
+    <hyperlink ref="D24" r:id="rId6" xr:uid="{0FC2B590-1D30-4B0E-B4F3-91D561480473}"/>
+    <hyperlink ref="E24" r:id="rId7" xr:uid="{BAE97140-2FD1-4239-B61E-9DD90968997C}"/>
+    <hyperlink ref="H19" r:id="rId8" xr:uid="{021BD0C3-71A2-4569-95D3-2F9A7C9A691E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified optimal size/mass ratio
</commit_message>
<xml_diff>
--- a/OptimSize.xlsx
+++ b/OptimSize.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Size_Consumption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA5E9D9-6C78-4A80-B131-A84BCCC9847D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D32B3A-E64C-4C48-BA22-72F5BC6EE28B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A77FD14E-277F-4AE2-BBD9-FAE0E9C9CB9C}"/>
   </bookViews>
@@ -512,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EF37AE-1B1C-479B-B90C-A1B96650C98F}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -689,7 +689,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -712,7 +712,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -730,7 +730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>132</v>
       </c>
@@ -741,7 +741,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>155</v>
       </c>
@@ -752,7 +752,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>182</v>
       </c>
@@ -763,7 +763,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>217</v>
       </c>
@@ -774,7 +774,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
         <v>35</v>
       </c>
@@ -785,7 +785,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>237</v>
       </c>
@@ -813,8 +813,16 @@
       <c r="I26">
         <v>159</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <f>AVERAGE(B26:J26)</f>
+        <v>166.25</v>
+      </c>
+      <c r="L26">
+        <f>K26*0.07</f>
+        <v>11.637500000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>

</xml_diff>